<commit_message>
Gestione: finito check accessibilità
</commit_message>
<xml_diff>
--- a/Assets/Notes and Utilities/GAG-checklist.xlsx
+++ b/Assets/Notes and Utilities/GAG-checklist.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgettiVideogiochi\ProgettiUnity\LaRiscrittora_Prototipo\Assets\Notes and Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BA1572-7BDC-4AEB-AB51-B24E0E02E1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CC806C-6F07-433A-8186-2BD23D08F87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-2370" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$174</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="184">
   <si>
     <t>Guideline</t>
   </si>
@@ -414,16 +417,7 @@
     <t>Non necessario</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Non abbiamo colori di testo, solo formattazioni</t>
-  </si>
-  <si>
-    <t>Non abbiamo elementi 3d</t>
-  </si>
-  <si>
-    <t>Non abbiamo il VR</t>
   </si>
   <si>
     <t>Obiettivi</t>
@@ -467,9 +461,6 @@
     <t>Abilitare/disabilitare animazioni del background per leggibilità schermo</t>
   </si>
   <si>
-    <t>Text to voice option (evitando le AI se riusciamo)?</t>
-  </si>
-  <si>
     <t>Filtro bianco o nero regolabile sul background https://gameaccessibilityguidelines.com/epic-eric-contrast-settings/</t>
   </si>
   <si>
@@ -482,16 +473,139 @@
     <t>Capire come rendere chiara parte di interattività</t>
   </si>
   <si>
-    <t>No manuali</t>
-  </si>
-  <si>
     <t>Due controlli diversi tra effetti audio e musica</t>
   </si>
   <si>
-    <t>No problema</t>
-  </si>
-  <si>
     <t>Valutare inserimento opzione?</t>
+  </si>
+  <si>
+    <t>Nei piani</t>
+  </si>
+  <si>
+    <t>Elemento non presente nel progetto</t>
+  </si>
+  <si>
+    <t>Non so sei il text to voice o screenreader possa fare o meno qualcosa del genere</t>
+  </si>
+  <si>
+    <t>Text to voice option (evitando le AI se riusciamo)? Screenreader</t>
+  </si>
+  <si>
+    <t>Sarebbe interessante, non so se sia fattibile sfruttando tutto il discorso di screenreading: le descrizione date dal fungo a quel punto sarebbero pensate per dare info sul contesto (e così il testo letto e quello da audiare sarebbero lo stesso).</t>
+  </si>
+  <si>
+    <t>Da fare</t>
+  </si>
+  <si>
+    <t>Da valutare? In generale l'audio qui è sempre d'accompagnamento, non narrativo.</t>
+  </si>
+  <si>
+    <t>Interessante, non so se e come sia fattibile.</t>
+  </si>
+  <si>
+    <t>Elemento non necessario (no voice over o simili)</t>
+  </si>
+  <si>
+    <t>Da inserire (sia su Steam/itch che nelle comunicazioni ad hoc sui social)</t>
+  </si>
+  <si>
+    <t>Da inserire (la mia speranza di fare tutto diegetico svanisce)</t>
+  </si>
+  <si>
+    <t>C'è, ma non impatta l'accessibilità</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Super</t>
+  </si>
+  <si>
+    <t>Da inserire (essendo sostanzialmente un vedo/non vedo stat la vedo easy)</t>
+  </si>
+  <si>
+    <t>Da capire come ma sì</t>
+  </si>
+  <si>
+    <t>Non impattante</t>
+  </si>
+  <si>
+    <t>Sarebbe la parte anarchist in teoria</t>
+  </si>
+  <si>
+    <t>Non fattibile</t>
+  </si>
+  <si>
+    <t>Riflessione in altro punto</t>
+  </si>
+  <si>
+    <t>Potrebbero esserci dei servizi già sfruttabili attraverso windows, ma non ho capito quanto e come: https://gameaccessibilityguidelines.com/ensure-screenreader-support-including-menus-installers/ e https://learn.microsoft.com/en-us/shows/gdc-2017/gdc2017-009</t>
+  </si>
+  <si>
+    <t>Già di default nel progetto (un solo tasto)</t>
+  </si>
+  <si>
+    <t>Ha senso?</t>
+  </si>
+  <si>
+    <t>Già inserito in punto sotto</t>
+  </si>
+  <si>
+    <t>Già di default nel progetto</t>
+  </si>
+  <si>
+    <t>Da inserire</t>
+  </si>
+  <si>
+    <t>Non so se sia fattibile come cosa, tenendo conto che le tavole son disegnate con una certa logica.</t>
+  </si>
+  <si>
+    <t>Idem come sopra</t>
+  </si>
+  <si>
+    <t>Non avremo la versione ufficiale mobile</t>
+  </si>
+  <si>
+    <t>Con un solo bottone è già una cosa di default?</t>
+  </si>
+  <si>
+    <t>Ho l'impressione che lo stile del gioco non lo preveda sempre.</t>
+  </si>
+  <si>
+    <t>Riflessione da fare in generale su informazioni date per gestire il gioco</t>
+  </si>
+  <si>
+    <t>Riflessione generale da fare</t>
+  </si>
+  <si>
+    <t>Non dovrebbe essere necessario. Eventualmente mostrare icona tasto a riavvio gioco?</t>
+  </si>
+  <si>
+    <t>Non credo sia evitabile</t>
+  </si>
+  <si>
+    <t>Previsto (scheda personagge)</t>
+  </si>
+  <si>
+    <t>Non possibile</t>
+  </si>
+  <si>
+    <t>Già indicato in altro punto</t>
+  </si>
+  <si>
+    <t>Salvataggio unico (?)</t>
+  </si>
+  <si>
+    <t>Da valutare</t>
+  </si>
+  <si>
+    <t>Usare bold (già nel tutorial)</t>
+  </si>
+  <si>
+    <t>Creare un log?</t>
+  </si>
+  <si>
+    <t>Fattibile?</t>
   </si>
 </sst>
 </file>
@@ -569,7 +683,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +693,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -623,6 +755,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -946,11 +1087,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -972,7 +1114,7 @@
         <v>127</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>125</v>
@@ -984,26 +1126,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="21" customHeight="1">
+    <row r="2" spans="1:6" ht="21" hidden="1" customHeight="1">
       <c r="A2" s="3"/>
       <c r="D2" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="38.25">
+    <row r="3" spans="1:6" ht="38.25" hidden="1">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" hidden="1">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" hidden="1">
       <c r="A5"/>
     </row>
-    <row r="6" spans="1:6" ht="27">
+    <row r="6" spans="1:6" ht="27" hidden="1">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -1012,31 +1154,46 @@
       <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30">
+      <c r="C7" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" hidden="1">
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="30">
+      <c r="B8" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" hidden="1">
       <c r="A9" s="6" t="s">
         <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="30">
+      <c r="C10" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" hidden="1">
       <c r="A11" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="B11" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1">
       <c r="A12"/>
     </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" ht="27">
+    <row r="13" spans="1:6" s="8" customFormat="1" ht="27" hidden="1">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -1047,159 +1204,223 @@
       <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="30">
+      <c r="C14" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" hidden="1">
       <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="45">
+      <c r="B15" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" hidden="1">
       <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="60">
+      <c r="B16" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60" hidden="1">
       <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="B17" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" hidden="1">
       <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="B18" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" hidden="1">
       <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30">
       <c r="A20" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" hidden="1">
       <c r="A21" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="B21" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30">
       <c r="A22" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" hidden="1">
       <c r="A24" s="6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="B24" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" hidden="1">
       <c r="A25" s="6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="B25" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" hidden="1">
       <c r="A26"/>
     </row>
-    <row r="27" spans="1:2" ht="27">
+    <row r="27" spans="1:3" ht="27" hidden="1">
       <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:3" hidden="1">
       <c r="A28" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="45">
+      <c r="B28" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" hidden="1">
       <c r="A29" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="30">
+      <c r="B29" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30">
       <c r="A30" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="30">
+      <c r="C30" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30">
       <c r="A31" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" hidden="1">
       <c r="A32"/>
     </row>
-    <row r="33" spans="1:3" ht="38.25">
+    <row r="33" spans="1:3" ht="38.25" hidden="1">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" hidden="1">
       <c r="A34" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="8" customFormat="1">
+    <row r="35" spans="1:3" s="8" customFormat="1" hidden="1">
       <c r="A35"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" ht="27">
+    <row r="36" spans="1:3" ht="27" hidden="1">
       <c r="A36" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30">
+    <row r="37" spans="1:3" ht="30" hidden="1">
       <c r="A37" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="B37" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" hidden="1">
       <c r="A38" s="6" t="s">
         <v>43</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="C39" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" hidden="1">
       <c r="A40" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="B40" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" hidden="1">
       <c r="A41" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" s="8" customFormat="1">
+      <c r="B41" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="8" customFormat="1" hidden="1">
       <c r="A42" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" s="8" customFormat="1">
+    <row r="43" spans="1:3" s="8" customFormat="1" hidden="1">
       <c r="A43" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" hidden="1">
       <c r="A44"/>
     </row>
-    <row r="45" spans="1:3" s="8" customFormat="1" ht="27">
+    <row r="45" spans="1:3" s="8" customFormat="1" ht="27" hidden="1">
       <c r="A45" s="4" t="s">
         <v>8</v>
       </c>
@@ -1210,183 +1431,249 @@
       <c r="A46" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="C46" s="11" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="C47" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="30">
       <c r="A48" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" ht="30">
+      <c r="C48" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30" hidden="1">
       <c r="A49" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="C50" s="12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" ht="30">
+      <c r="C51" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="30" hidden="1">
       <c r="A52" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" hidden="1">
       <c r="A53" s="6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" hidden="1">
       <c r="A54" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" hidden="1">
       <c r="A55" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" hidden="1">
       <c r="A56" s="6" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" ht="30">
+      <c r="B56" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30" hidden="1">
       <c r="A57" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" ht="30">
+      <c r="B57" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="30" hidden="1">
       <c r="A58" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" hidden="1">
       <c r="A59" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" ht="30">
+      <c r="B59" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="30">
       <c r="A60" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="C60" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="C61" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" hidden="1">
       <c r="A62"/>
     </row>
-    <row r="63" spans="1:1" ht="27">
+    <row r="63" spans="1:3" ht="27" hidden="1">
       <c r="A63" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:3" hidden="1">
       <c r="A64" s="6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="30">
+      <c r="B64" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30" hidden="1">
       <c r="A65" s="6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
+      <c r="B65" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" hidden="1">
       <c r="A66" s="6" t="s">
         <v>64</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="6" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
+      <c r="C67" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" hidden="1">
       <c r="A68" s="6" t="s">
         <v>66</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
+      <c r="C69" s="10" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" hidden="1">
       <c r="A70"/>
     </row>
-    <row r="71" spans="1:3" ht="38.25">
+    <row r="71" spans="1:3" ht="38.25" hidden="1">
       <c r="A71" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" hidden="1">
       <c r="A72"/>
     </row>
-    <row r="73" spans="1:3" ht="27">
+    <row r="73" spans="1:3" ht="27" hidden="1">
       <c r="A73" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" hidden="1">
       <c r="A74" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" s="8" customFormat="1" ht="30">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" s="8" customFormat="1" ht="30" hidden="1">
       <c r="A75" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" hidden="1">
       <c r="A76" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="30">
       <c r="A77" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>133</v>
+      <c r="C77" s="11" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="30">
       <c r="A78" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>134</v>
+      <c r="C78" s="11" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="30">
       <c r="A79" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>135</v>
+      <c r="C79" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:3" s="8" customFormat="1" ht="30">
@@ -1394,127 +1681,127 @@
         <v>25</v>
       </c>
       <c r="B80" s="1"/>
-      <c r="C80" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="C80" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" hidden="1">
       <c r="A81"/>
     </row>
-    <row r="82" spans="1:3" ht="27">
+    <row r="82" spans="1:3" ht="27" hidden="1">
       <c r="A82" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="30">
+    <row r="83" spans="1:3" ht="30" hidden="1">
       <c r="A83" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" s="8" customFormat="1" ht="45">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" s="8" customFormat="1" ht="45" hidden="1">
       <c r="A84" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="C84" s="1"/>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" hidden="1">
       <c r="A85" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="30">
       <c r="A86" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>137</v>
+      <c r="C86" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>138</v>
+      <c r="C87" s="10" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="30">
       <c r="A88" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>139</v>
+      <c r="C88" s="11" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="30">
       <c r="A89" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>140</v>
+      <c r="C89" s="10" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>141</v>
+      <c r="C90" s="11" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="30">
+      <c r="C91" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="30" hidden="1">
       <c r="A92" s="6" t="s">
         <v>79</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="30">
       <c r="A93" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="30">
+      <c r="C93" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="30" hidden="1">
       <c r="A94" s="6" t="s">
         <v>80</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="C95" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" hidden="1">
       <c r="A96"/>
     </row>
-    <row r="97" spans="1:3" ht="27">
+    <row r="97" spans="1:3" ht="27" hidden="1">
       <c r="A97" s="4" t="s">
         <v>15</v>
       </c>
@@ -1523,10 +1810,16 @@
       <c r="A98" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="99" spans="1:3">
+      <c r="C98" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" hidden="1">
       <c r="A99" s="6" t="s">
         <v>82</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:3" s="8" customFormat="1" ht="30">
@@ -1534,26 +1827,40 @@
         <v>83</v>
       </c>
       <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="C100" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" hidden="1">
       <c r="A101" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="B101" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" hidden="1">
       <c r="A102" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="60">
+      <c r="B102" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="60" hidden="1">
       <c r="A103" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="104" spans="1:3">
+      <c r="B103" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="75">
       <c r="A104" s="6" t="s">
         <v>87</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="105" spans="1:3" s="8" customFormat="1">
@@ -1561,262 +1868,356 @@
         <v>88</v>
       </c>
       <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-    </row>
-    <row r="106" spans="1:3">
+      <c r="C105" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" hidden="1">
       <c r="A106" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
+      <c r="B106" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="60">
       <c r="A107" s="6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="C107" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" hidden="1">
       <c r="A108"/>
     </row>
-    <row r="109" spans="1:3" ht="38.25">
+    <row r="109" spans="1:3" ht="38.25" hidden="1">
       <c r="A109" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" hidden="1">
       <c r="A110"/>
     </row>
-    <row r="111" spans="1:3" ht="27">
+    <row r="111" spans="1:3" ht="27" hidden="1">
       <c r="A111" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" hidden="1">
       <c r="A112" s="6" t="s">
         <v>113</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="30">
       <c r="A113" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="114" spans="1:3">
+      <c r="C113" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" hidden="1">
       <c r="A114" s="6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" ht="30">
+      <c r="B114" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="30" hidden="1">
       <c r="A115" s="6" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="116" spans="1:3">
+      <c r="B115" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" hidden="1">
       <c r="A116"/>
     </row>
-    <row r="117" spans="1:3" ht="27">
+    <row r="117" spans="1:3" ht="27" hidden="1">
       <c r="A117" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:3" s="8" customFormat="1">
+    <row r="118" spans="1:3" s="8" customFormat="1" hidden="1">
       <c r="A118" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B118" s="1"/>
+      <c r="B118" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="C118" s="1"/>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" hidden="1">
       <c r="A119" s="6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" ht="30">
+      <c r="B119" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="30" hidden="1">
       <c r="A120" s="6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="121" spans="1:3">
+      <c r="B120" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="30">
       <c r="A121" s="6" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="122" spans="1:3">
+      <c r="C121" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" hidden="1">
       <c r="A122" s="6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="123" spans="1:3">
+      <c r="B122" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" hidden="1">
       <c r="A123" s="6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="124" spans="1:3">
+      <c r="B123" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" hidden="1">
       <c r="A124" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="125" spans="1:3">
+      <c r="B124" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" hidden="1">
       <c r="A125" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" ht="45">
+      <c r="B125" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="30" hidden="1">
       <c r="A126" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" ht="45">
+      <c r="B126" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="45" hidden="1">
       <c r="A127" s="6" t="s">
         <v>97</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="C128" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" hidden="1">
       <c r="A129"/>
     </row>
-    <row r="130" spans="1:1" ht="27">
+    <row r="130" spans="1:2" ht="27" hidden="1">
       <c r="A130" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="30">
+    <row r="131" spans="1:2" ht="30" hidden="1">
       <c r="A131" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="B131" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="30" hidden="1">
       <c r="A132" s="6" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="B132" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" hidden="1">
       <c r="A133" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="B133" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" hidden="1">
       <c r="A134"/>
     </row>
-    <row r="135" spans="1:1" ht="38.25">
+    <row r="135" spans="1:2" ht="38.25" hidden="1">
       <c r="A135" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:2" hidden="1">
       <c r="A136"/>
     </row>
-    <row r="137" spans="1:1" ht="27">
+    <row r="137" spans="1:2" ht="27" hidden="1">
       <c r="A137" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:1" ht="30">
+    <row r="138" spans="1:2" ht="30" hidden="1">
       <c r="A138" s="6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="B138" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" hidden="1">
       <c r="A139"/>
     </row>
-    <row r="140" spans="1:1" ht="27">
+    <row r="140" spans="1:2" ht="27" hidden="1">
       <c r="A140" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="45">
+    <row r="141" spans="1:2" ht="30" hidden="1">
       <c r="A141" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="142" spans="1:1">
+      <c r="B141" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" hidden="1">
       <c r="A142" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="B142" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" hidden="1">
       <c r="A143" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" ht="30">
+      <c r="B143" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="30" hidden="1">
       <c r="A144" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="B144" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" hidden="1">
       <c r="A145"/>
     </row>
-    <row r="146" spans="1:3" ht="27">
+    <row r="146" spans="1:3" ht="27" hidden="1">
       <c r="A146" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="30">
+    <row r="147" spans="1:3" ht="30" hidden="1">
       <c r="A147" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" s="8" customFormat="1">
+      <c r="B147" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" s="8" customFormat="1" hidden="1">
       <c r="A148" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B148" s="1"/>
+      <c r="B148" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="C148" s="1"/>
     </row>
-    <row r="149" spans="1:3" s="8" customFormat="1">
+    <row r="149" spans="1:3" s="8" customFormat="1" hidden="1">
       <c r="A149" s="6"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="1:3" ht="38.25">
+    <row r="150" spans="1:3" ht="38.25" hidden="1">
       <c r="A150" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" hidden="1">
       <c r="A151"/>
     </row>
-    <row r="152" spans="1:3" ht="27">
+    <row r="152" spans="1:3" ht="27" hidden="1">
       <c r="A152" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" ht="30">
       <c r="A153" s="6" t="s">
         <v>5</v>
+      </c>
+      <c r="C153" s="11" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="6" t="s">
         <v>120</v>
       </c>
+      <c r="C154" s="11" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="155" spans="1:3" s="8" customFormat="1">
       <c r="A155" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
+      <c r="C155" s="11" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="C156" s="11" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="157" spans="1:3" s="8" customFormat="1">
       <c r="A157" s="6" t="s">
         <v>121</v>
       </c>
       <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
-    </row>
-    <row r="158" spans="1:3">
+      <c r="C157" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" hidden="1">
       <c r="A158"/>
     </row>
-    <row r="159" spans="1:3" ht="27">
+    <row r="159" spans="1:3" ht="27" hidden="1">
       <c r="A159" s="4" t="s">
         <v>8</v>
       </c>
@@ -1825,72 +2226,113 @@
       <c r="A160" s="6" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" ht="30">
+      <c r="C160" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="30">
       <c r="A161" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" ht="30">
+      <c r="C161" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="30" hidden="1">
       <c r="A162" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="163" spans="1:1">
+      <c r="B162" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" hidden="1">
       <c r="A163" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="B163" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" hidden="1">
       <c r="A164" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="B164" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" hidden="1">
       <c r="A165" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" ht="45">
+      <c r="B165" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="45" hidden="1">
       <c r="A166" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" ht="30">
+      <c r="B166" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="30">
       <c r="A167" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="168" spans="1:1">
+      <c r="C167" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" hidden="1">
       <c r="A168"/>
     </row>
-    <row r="169" spans="1:1" ht="27">
+    <row r="169" spans="1:3" ht="27" hidden="1">
       <c r="A169" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:1" ht="45">
+    <row r="170" spans="1:3" ht="45">
       <c r="A170" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" ht="30">
+      <c r="C170" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="30">
       <c r="A171" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="172" spans="1:1">
+      <c r="C171" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" hidden="1">
       <c r="A172" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" ht="56.25">
+      <c r="B172" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" hidden="1"/>
+    <row r="174" spans="1:3" ht="56.25" hidden="1">
       <c r="A174" s="9" t="s">
         <v>126</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A78:B78 D78:AB78 A1:AB77 A79:AB1514">
+  <autoFilter ref="A1:F174" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A78:B78 D78:AB78 A79:AB1514 A1:AB7 D8:AB8 A8:B8 A9:AB77">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>INDIRECT("b"&amp;ROW())="No"</formula>
     </cfRule>

</xml_diff>